<commit_message>
finish the first 3 sections
</commit_message>
<xml_diff>
--- a/output/datos_serializados.xlsx
+++ b/output/datos_serializados.xlsx
@@ -525,14 +525,14 @@
       <c r="C2" t="n">
         <v>1</v>
       </c>
-      <c r="D2" t="b">
-        <v>1</v>
+      <c r="D2" t="n">
+        <v>0</v>
       </c>
       <c r="E2" t="n">
         <v>1</v>
       </c>
-      <c r="F2" t="b">
-        <v>1</v>
+      <c r="F2" t="n">
+        <v>0</v>
       </c>
       <c r="G2" t="n">
         <v>-2</v>
@@ -550,8 +550,8 @@
           <t>[1]</t>
         </is>
       </c>
-      <c r="K2" t="b">
-        <v>0</v>
+      <c r="K2" t="n">
+        <v>1</v>
       </c>
       <c r="L2" t="n">
         <v>1</v>
@@ -577,14 +577,14 @@
       <c r="C3" t="n">
         <v>1</v>
       </c>
-      <c r="D3" t="b">
-        <v>1</v>
+      <c r="D3" t="n">
+        <v>0</v>
       </c>
       <c r="E3" t="n">
         <v>1</v>
       </c>
-      <c r="F3" t="b">
-        <v>1</v>
+      <c r="F3" t="n">
+        <v>0</v>
       </c>
       <c r="G3" t="n">
         <v>-1</v>
@@ -602,7 +602,7 @@
           <t>[1]</t>
         </is>
       </c>
-      <c r="K3" t="b">
+      <c r="K3" t="n">
         <v>0</v>
       </c>
       <c r="L3" t="n">
@@ -629,14 +629,14 @@
       <c r="C4" t="n">
         <v>1</v>
       </c>
-      <c r="D4" t="b">
-        <v>1</v>
+      <c r="D4" t="n">
+        <v>0</v>
       </c>
       <c r="E4" t="n">
         <v>1</v>
       </c>
-      <c r="F4" t="b">
-        <v>1</v>
+      <c r="F4" t="n">
+        <v>0</v>
       </c>
       <c r="G4" t="n">
         <v>-1</v>
@@ -654,7 +654,7 @@
           <t>[1]</t>
         </is>
       </c>
-      <c r="K4" t="b">
+      <c r="K4" t="n">
         <v>0</v>
       </c>
       <c r="L4" t="n">
@@ -681,14 +681,14 @@
       <c r="C5" t="n">
         <v>1</v>
       </c>
-      <c r="D5" t="b">
-        <v>1</v>
+      <c r="D5" t="n">
+        <v>0</v>
       </c>
       <c r="E5" t="n">
         <v>0</v>
       </c>
-      <c r="F5" t="b">
-        <v>1</v>
+      <c r="F5" t="n">
+        <v>0</v>
       </c>
       <c r="G5" t="n">
         <v>-1</v>
@@ -706,8 +706,8 @@
           <t>[0, 2]</t>
         </is>
       </c>
-      <c r="K5" t="b">
-        <v>0</v>
+      <c r="K5" t="n">
+        <v>1</v>
       </c>
       <c r="L5" t="n">
         <v>1</v>
@@ -733,14 +733,14 @@
       <c r="C6" t="n">
         <v>0</v>
       </c>
-      <c r="D6" t="b">
-        <v>1</v>
+      <c r="D6" t="n">
+        <v>0</v>
       </c>
       <c r="E6" t="n">
         <v>1</v>
       </c>
-      <c r="F6" t="b">
-        <v>1</v>
+      <c r="F6" t="n">
+        <v>0</v>
       </c>
       <c r="G6" t="n">
         <v>-1</v>
@@ -758,7 +758,7 @@
           <t>[1, 2]</t>
         </is>
       </c>
-      <c r="K6" t="b">
+      <c r="K6" t="n">
         <v>0</v>
       </c>
       <c r="L6" t="n">
@@ -785,14 +785,14 @@
       <c r="C7" t="n">
         <v>1</v>
       </c>
-      <c r="D7" t="b">
-        <v>1</v>
+      <c r="D7" t="n">
+        <v>0</v>
       </c>
       <c r="E7" t="n">
         <v>-1</v>
       </c>
-      <c r="F7" t="b">
-        <v>1</v>
+      <c r="F7" t="n">
+        <v>0</v>
       </c>
       <c r="G7" t="n">
         <v>-1</v>
@@ -810,7 +810,7 @@
           <t>[2, 3]</t>
         </is>
       </c>
-      <c r="K7" t="b">
+      <c r="K7" t="n">
         <v>0</v>
       </c>
       <c r="L7" t="n">
@@ -837,14 +837,14 @@
       <c r="C8" t="n">
         <v>0</v>
       </c>
-      <c r="D8" t="b">
-        <v>1</v>
+      <c r="D8" t="n">
+        <v>0</v>
       </c>
       <c r="E8" t="n">
         <v>-1</v>
       </c>
-      <c r="F8" t="b">
-        <v>1</v>
+      <c r="F8" t="n">
+        <v>0</v>
       </c>
       <c r="G8" t="n">
         <v>-1</v>
@@ -862,7 +862,7 @@
           <t>[0, 2]</t>
         </is>
       </c>
-      <c r="K8" t="b">
+      <c r="K8" t="n">
         <v>0</v>
       </c>
       <c r="L8" t="n">
@@ -889,14 +889,14 @@
       <c r="C9" t="n">
         <v>0</v>
       </c>
-      <c r="D9" t="b">
-        <v>1</v>
+      <c r="D9" t="n">
+        <v>0</v>
       </c>
       <c r="E9" t="n">
         <v>1</v>
       </c>
-      <c r="F9" t="b">
-        <v>1</v>
+      <c r="F9" t="n">
+        <v>0</v>
       </c>
       <c r="G9" t="n">
         <v>-1</v>
@@ -914,8 +914,8 @@
           <t>[0, 2]</t>
         </is>
       </c>
-      <c r="K9" t="b">
-        <v>0</v>
+      <c r="K9" t="n">
+        <v>1</v>
       </c>
       <c r="L9" t="n">
         <v>-1</v>
@@ -941,14 +941,14 @@
       <c r="C10" t="n">
         <v>1</v>
       </c>
-      <c r="D10" t="b">
-        <v>1</v>
+      <c r="D10" t="n">
+        <v>0</v>
       </c>
       <c r="E10" t="n">
         <v>1</v>
       </c>
-      <c r="F10" t="b">
-        <v>1</v>
+      <c r="F10" t="n">
+        <v>0</v>
       </c>
       <c r="G10" t="n">
         <v>1</v>
@@ -966,8 +966,8 @@
           <t>[0, 1, 2, 3]</t>
         </is>
       </c>
-      <c r="K10" t="b">
-        <v>0</v>
+      <c r="K10" t="n">
+        <v>1</v>
       </c>
       <c r="L10" t="n">
         <v>0</v>
@@ -993,14 +993,14 @@
       <c r="C11" t="n">
         <v>0</v>
       </c>
-      <c r="D11" t="b">
-        <v>1</v>
+      <c r="D11" t="n">
+        <v>0</v>
       </c>
       <c r="E11" t="n">
         <v>1</v>
       </c>
-      <c r="F11" t="b">
-        <v>1</v>
+      <c r="F11" t="n">
+        <v>0</v>
       </c>
       <c r="G11" t="n">
         <v>1</v>
@@ -1018,8 +1018,8 @@
           <t>[0]</t>
         </is>
       </c>
-      <c r="K11" t="b">
-        <v>0</v>
+      <c r="K11" t="n">
+        <v>1</v>
       </c>
       <c r="L11" t="n">
         <v>0</v>
@@ -1045,14 +1045,14 @@
       <c r="C12" t="n">
         <v>1</v>
       </c>
-      <c r="D12" t="b">
-        <v>1</v>
+      <c r="D12" t="n">
+        <v>0</v>
       </c>
       <c r="E12" t="n">
         <v>0</v>
       </c>
-      <c r="F12" t="b">
-        <v>1</v>
+      <c r="F12" t="n">
+        <v>0</v>
       </c>
       <c r="G12" t="n">
         <v>-1</v>
@@ -1070,8 +1070,8 @@
           <t>[0, 2]</t>
         </is>
       </c>
-      <c r="K12" t="b">
-        <v>0</v>
+      <c r="K12" t="n">
+        <v>1</v>
       </c>
       <c r="L12" t="n">
         <v>0</v>
@@ -1097,14 +1097,14 @@
       <c r="C13" t="n">
         <v>1</v>
       </c>
-      <c r="D13" t="b">
-        <v>1</v>
+      <c r="D13" t="n">
+        <v>0</v>
       </c>
       <c r="E13" t="n">
         <v>1</v>
       </c>
-      <c r="F13" t="b">
-        <v>1</v>
+      <c r="F13" t="n">
+        <v>0</v>
       </c>
       <c r="G13" t="n">
         <v>-1</v>
@@ -1122,8 +1122,8 @@
           <t>[0, 1, 2, 3]</t>
         </is>
       </c>
-      <c r="K13" t="b">
-        <v>0</v>
+      <c r="K13" t="n">
+        <v>1</v>
       </c>
       <c r="L13" t="n">
         <v>-1</v>
@@ -1149,14 +1149,14 @@
       <c r="C14" t="n">
         <v>1</v>
       </c>
-      <c r="D14" t="b">
-        <v>1</v>
+      <c r="D14" t="n">
+        <v>0</v>
       </c>
       <c r="E14" t="n">
         <v>1</v>
       </c>
-      <c r="F14" t="b">
-        <v>1</v>
+      <c r="F14" t="n">
+        <v>0</v>
       </c>
       <c r="G14" t="n">
         <v>0</v>
@@ -1174,8 +1174,8 @@
           <t>[0, 1, 3]</t>
         </is>
       </c>
-      <c r="K14" t="b">
-        <v>0</v>
+      <c r="K14" t="n">
+        <v>1</v>
       </c>
       <c r="L14" t="n">
         <v>-2</v>
@@ -1201,14 +1201,14 @@
       <c r="C15" t="n">
         <v>0</v>
       </c>
-      <c r="D15" t="b">
-        <v>1</v>
+      <c r="D15" t="n">
+        <v>0</v>
       </c>
       <c r="E15" t="n">
         <v>1</v>
       </c>
-      <c r="F15" t="b">
-        <v>1</v>
+      <c r="F15" t="n">
+        <v>0</v>
       </c>
       <c r="G15" t="n">
         <v>1</v>
@@ -1226,8 +1226,8 @@
           <t>[0, 2, 3]</t>
         </is>
       </c>
-      <c r="K15" t="b">
-        <v>0</v>
+      <c r="K15" t="n">
+        <v>1</v>
       </c>
       <c r="L15" t="n">
         <v>-2</v>
@@ -1253,14 +1253,14 @@
       <c r="C16" t="n">
         <v>1</v>
       </c>
-      <c r="D16" t="b">
-        <v>1</v>
+      <c r="D16" t="n">
+        <v>0</v>
       </c>
       <c r="E16" t="n">
         <v>1</v>
       </c>
-      <c r="F16" t="b">
-        <v>1</v>
+      <c r="F16" t="n">
+        <v>0</v>
       </c>
       <c r="G16" t="n">
         <v>-1</v>
@@ -1278,8 +1278,8 @@
           <t>[0, 1]</t>
         </is>
       </c>
-      <c r="K16" t="b">
-        <v>0</v>
+      <c r="K16" t="n">
+        <v>1</v>
       </c>
       <c r="L16" t="n">
         <v>0</v>
@@ -1305,14 +1305,14 @@
       <c r="C17" t="n">
         <v>0</v>
       </c>
-      <c r="D17" t="b">
-        <v>1</v>
+      <c r="D17" t="n">
+        <v>0</v>
       </c>
       <c r="E17" t="n">
         <v>1</v>
       </c>
-      <c r="F17" t="b">
-        <v>1</v>
+      <c r="F17" t="n">
+        <v>0</v>
       </c>
       <c r="G17" t="n">
         <v>-1</v>
@@ -1330,7 +1330,7 @@
           <t>[1]</t>
         </is>
       </c>
-      <c r="K17" t="b">
+      <c r="K17" t="n">
         <v>0</v>
       </c>
       <c r="L17" t="n">
@@ -1357,14 +1357,14 @@
       <c r="C18" t="n">
         <v>1</v>
       </c>
-      <c r="D18" t="b">
-        <v>1</v>
+      <c r="D18" t="n">
+        <v>0</v>
       </c>
       <c r="E18" t="n">
         <v>0</v>
       </c>
-      <c r="F18" t="b">
-        <v>1</v>
+      <c r="F18" t="n">
+        <v>0</v>
       </c>
       <c r="G18" t="n">
         <v>0</v>
@@ -1382,8 +1382,8 @@
           <t>[0]</t>
         </is>
       </c>
-      <c r="K18" t="b">
-        <v>0</v>
+      <c r="K18" t="n">
+        <v>1</v>
       </c>
       <c r="L18" t="n">
         <v>-2</v>
@@ -1409,14 +1409,14 @@
       <c r="C19" t="n">
         <v>1</v>
       </c>
-      <c r="D19" t="b">
-        <v>1</v>
+      <c r="D19" t="n">
+        <v>0</v>
       </c>
       <c r="E19" t="n">
         <v>1</v>
       </c>
-      <c r="F19" t="b">
-        <v>1</v>
+      <c r="F19" t="n">
+        <v>0</v>
       </c>
       <c r="G19" t="n">
         <v>1</v>
@@ -1434,8 +1434,8 @@
           <t>[0, 1, 3]</t>
         </is>
       </c>
-      <c r="K19" t="b">
-        <v>0</v>
+      <c r="K19" t="n">
+        <v>1</v>
       </c>
       <c r="L19" t="n">
         <v>-2</v>
@@ -1461,14 +1461,14 @@
       <c r="C20" t="n">
         <v>1</v>
       </c>
-      <c r="D20" t="b">
-        <v>1</v>
+      <c r="D20" t="n">
+        <v>0</v>
       </c>
       <c r="E20" t="n">
         <v>1</v>
       </c>
-      <c r="F20" t="b">
-        <v>1</v>
+      <c r="F20" t="n">
+        <v>0</v>
       </c>
       <c r="G20" t="n">
         <v>-1</v>
@@ -1486,8 +1486,8 @@
           <t>[1, 3]</t>
         </is>
       </c>
-      <c r="K20" t="b">
-        <v>0</v>
+      <c r="K20" t="n">
+        <v>1</v>
       </c>
       <c r="L20" t="n">
         <v>-2</v>
@@ -1513,14 +1513,14 @@
       <c r="C21" t="n">
         <v>0</v>
       </c>
-      <c r="D21" t="b">
-        <v>1</v>
+      <c r="D21" t="n">
+        <v>0</v>
       </c>
       <c r="E21" t="n">
         <v>0</v>
       </c>
-      <c r="F21" t="b">
-        <v>1</v>
+      <c r="F21" t="n">
+        <v>0</v>
       </c>
       <c r="G21" t="n">
         <v>-2</v>
@@ -1538,8 +1538,8 @@
           <t>[0]</t>
         </is>
       </c>
-      <c r="K21" t="b">
-        <v>0</v>
+      <c r="K21" t="n">
+        <v>1</v>
       </c>
       <c r="L21" t="n">
         <v>0</v>
@@ -1565,14 +1565,14 @@
       <c r="C22" t="n">
         <v>0</v>
       </c>
-      <c r="D22" t="b">
-        <v>0</v>
+      <c r="D22" t="n">
+        <v>1</v>
       </c>
       <c r="E22" t="n">
         <v>0</v>
       </c>
-      <c r="F22" t="b">
-        <v>1</v>
+      <c r="F22" t="n">
+        <v>0</v>
       </c>
       <c r="G22" t="n">
         <v>-2</v>
@@ -1590,7 +1590,7 @@
           <t>[2]</t>
         </is>
       </c>
-      <c r="K22" t="b">
+      <c r="K22" t="n">
         <v>0</v>
       </c>
       <c r="L22" t="n">
@@ -1617,14 +1617,14 @@
       <c r="C23" t="n">
         <v>0</v>
       </c>
-      <c r="D23" t="b">
-        <v>1</v>
+      <c r="D23" t="n">
+        <v>0</v>
       </c>
       <c r="E23" t="n">
         <v>1</v>
       </c>
-      <c r="F23" t="b">
-        <v>1</v>
+      <c r="F23" t="n">
+        <v>0</v>
       </c>
       <c r="G23" t="n">
         <v>1</v>
@@ -1642,8 +1642,8 @@
           <t>[1]</t>
         </is>
       </c>
-      <c r="K23" t="b">
-        <v>0</v>
+      <c r="K23" t="n">
+        <v>1</v>
       </c>
       <c r="L23" t="n">
         <v>-1</v>
@@ -1669,14 +1669,14 @@
       <c r="C24" t="n">
         <v>0</v>
       </c>
-      <c r="D24" t="b">
-        <v>1</v>
+      <c r="D24" t="n">
+        <v>0</v>
       </c>
       <c r="E24" t="n">
         <v>1</v>
       </c>
-      <c r="F24" t="b">
-        <v>1</v>
+      <c r="F24" t="n">
+        <v>0</v>
       </c>
       <c r="G24" t="n">
         <v>1</v>
@@ -1694,8 +1694,8 @@
           <t>[0, 1, 2]</t>
         </is>
       </c>
-      <c r="K24" t="b">
-        <v>0</v>
+      <c r="K24" t="n">
+        <v>1</v>
       </c>
       <c r="L24" t="n">
         <v>1</v>

</xml_diff>